<commit_message>
update review for final
</commit_message>
<xml_diff>
--- a/_PowerPoints/2nd Semester/Unit 8 Bridge Building/A3 Projects/Summative Sheet Bridge.xlsx
+++ b/_PowerPoints/2nd Semester/Unit 8 Bridge Building/A3 Projects/Summative Sheet Bridge.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="49">
   <si>
     <t xml:space="preserve">Used Classtime Appropriately </t>
   </si>
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -877,7 +877,9 @@
       <c r="D5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F5" s="1" t="s">
         <v>39</v>
       </c>
@@ -887,9 +889,13 @@
       <c r="H5" s="1">
         <v>40</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1">
+        <v>4</v>
+      </c>
       <c r="J5" s="3"/>
-      <c r="K5" s="16"/>
+      <c r="K5" s="16">
+        <v>4</v>
+      </c>
       <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -903,7 +909,9 @@
       <c r="D6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F6" s="1" t="s">
         <v>39</v>
       </c>
@@ -913,9 +921,13 @@
       <c r="H6" s="1">
         <v>40</v>
       </c>
-      <c r="I6" s="1"/>
+      <c r="I6" s="1">
+        <v>4</v>
+      </c>
       <c r="J6" s="3"/>
-      <c r="K6" s="16"/>
+      <c r="K6" s="16">
+        <v>4</v>
+      </c>
       <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -929,7 +941,9 @@
       <c r="D7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F7" s="1" t="s">
         <v>39</v>
       </c>
@@ -939,9 +953,13 @@
       <c r="H7" s="1">
         <v>40</v>
       </c>
-      <c r="I7" s="1"/>
+      <c r="I7" s="1">
+        <v>4</v>
+      </c>
       <c r="J7" s="3"/>
-      <c r="K7" s="16"/>
+      <c r="K7" s="16">
+        <v>4</v>
+      </c>
       <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -955,7 +973,9 @@
       <c r="D8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F8" s="1" t="s">
         <v>39</v>
       </c>
@@ -965,9 +985,13 @@
       <c r="H8" s="1">
         <v>40</v>
       </c>
-      <c r="I8" s="1"/>
+      <c r="I8" s="1">
+        <v>4</v>
+      </c>
       <c r="J8" s="3"/>
-      <c r="K8" s="16"/>
+      <c r="K8" s="16">
+        <v>4</v>
+      </c>
       <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -981,7 +1005,9 @@
       <c r="D9" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="18"/>
+      <c r="E9" s="18" t="s">
+        <v>39</v>
+      </c>
       <c r="F9" s="18" t="s">
         <v>39</v>
       </c>
@@ -991,9 +1017,13 @@
       <c r="H9" s="18">
         <v>40</v>
       </c>
-      <c r="I9" s="18"/>
+      <c r="I9" s="18">
+        <v>4</v>
+      </c>
       <c r="J9" s="3"/>
-      <c r="K9" s="16"/>
+      <c r="K9" s="16">
+        <v>3</v>
+      </c>
       <c r="L9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -1007,7 +1037,9 @@
       <c r="D10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F10" s="1" t="s">
         <v>39</v>
       </c>
@@ -1017,9 +1049,13 @@
       <c r="H10" s="1">
         <v>40</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1">
+        <v>4</v>
+      </c>
       <c r="J10" s="3"/>
-      <c r="K10" s="16"/>
+      <c r="K10" s="16">
+        <v>3</v>
+      </c>
       <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -1396,12 +1432,18 @@
         <v>41</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="3"/>
-      <c r="K24" s="16"/>
+      <c r="K24" s="16">
+        <v>2.5</v>
+      </c>
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -1416,12 +1458,18 @@
         <v>41</v>
       </c>
       <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="3"/>
-      <c r="K25" s="16"/>
+      <c r="K25" s="16">
+        <v>2.5</v>
+      </c>
       <c r="L25" s="8"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
@@ -1436,12 +1484,18 @@
         <v>41</v>
       </c>
       <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="3"/>
-      <c r="K26" s="16"/>
+      <c r="K26" s="16">
+        <v>2.5</v>
+      </c>
       <c r="L26" s="8"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
@@ -1456,12 +1510,18 @@
         <v>41</v>
       </c>
       <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="3"/>
-      <c r="K27" s="16"/>
+      <c r="K27" s="16">
+        <v>2.5</v>
+      </c>
       <c r="L27" s="8"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
@@ -1476,12 +1536,18 @@
         <v>41</v>
       </c>
       <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="3"/>
-      <c r="K28" s="16"/>
+      <c r="K28" s="16">
+        <v>2.5</v>
+      </c>
       <c r="L28" s="8"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.35">

</xml_diff>